<commit_message>
Update Pass/Fail of Main Window test cases
</commit_message>
<xml_diff>
--- a/Test related files/TestCases_MainWindow.xlsx
+++ b/Test related files/TestCases_MainWindow.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27203"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5B95F76-36AA-4C2C-B73F-CD4B58A5A208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF47E642-D02D-44CA-B0A8-A56B339A1EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -70,7 +70,13 @@
     <t>1+ entries in the database</t>
   </si>
   <si>
+    <t>Data List should contain contacts (Name, Phone No., Birth Date)</t>
+  </si>
+  <si>
     <t>Data List contains contacts (Name, Phone No., Birth Date)</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
   <si>
     <t>MW-002</t>
@@ -83,6 +89,9 @@
 2. Observe the Birth Date column in the Data List</t>
   </si>
   <si>
+    <t>Birth Date should be displayed in format YYYY-MM-DD</t>
+  </si>
+  <si>
     <t>Birth Date is displayed in format YYYY-MM-DD</t>
   </si>
   <si>
@@ -90,6 +99,9 @@
   </si>
   <si>
     <t>Data List fills the area between the top and buttons</t>
+  </si>
+  <si>
+    <t>Data List should fill the area between the top of the window and the buttons</t>
   </si>
   <si>
     <t>Data List fills the area between the top of the window and the buttons</t>
@@ -105,6 +117,9 @@
 2. Observe the buttons</t>
   </si>
   <si>
+    <t>Buttons should be the same sized at the bottom of the window</t>
+  </si>
+  <si>
     <t>Buttons are the same sized at the bottom of the window</t>
   </si>
   <si>
@@ -118,6 +133,9 @@
 2. Change the size of the window by dragging by the corner of the window with the mouse</t>
   </si>
   <si>
+    <t>Objects in the window should resize when the window is resized</t>
+  </si>
+  <si>
     <t>Objects in the window resize when the window is resized</t>
   </si>
   <si>
@@ -131,6 +149,9 @@
 2. Observe the "Delete" button</t>
   </si>
   <si>
+    <t>The "Delete" button should be disabled</t>
+  </si>
+  <si>
     <t>The "Delete" button is disabled</t>
   </si>
   <si>
@@ -142,6 +163,9 @@
   <si>
     <t>1. Open the Phonebook application
 2. Select the first contact in the list</t>
+  </si>
+  <si>
+    <t>The "Delete" button should becomes enabled</t>
   </si>
   <si>
     <t>The "Delete" button becomes enabled</t>
@@ -156,6 +180,9 @@
     <t>1. Open the Phonebook application
 2. Select the first contact in the list
 3. Press the "Delete" button</t>
+  </si>
+  <si>
+    <t>The selected contact should be deleted</t>
   </si>
   <si>
     <t>The selected contact is deleted</t>
@@ -985,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1040,35 +1067,43 @@
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="99.75" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="99.75" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -1076,104 +1111,128 @@
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="99.75" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="99.75" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="99.75" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="5"/>
       <c r="F7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="99.75" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="99.75" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H9">

</xml_diff>